<commit_message>
adding plots figure 1 and 2
</commit_message>
<xml_diff>
--- a/configuration.xlsx
+++ b/configuration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\GitHub\great-american-cities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\great-american-cities\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="280">
   <si>
     <t>City</t>
   </si>
@@ -866,6 +866,9 @@
   </si>
   <si>
     <t>No Buildings</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -901,12 +904,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1192,7 +1199,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A12"/>
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1745,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -1761,7 +1768,52 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1773,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,9 +1854,8 @@
       <c r="B2" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C2" s="1" t="e">
-        <f>VLOOKUP(A2,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C2" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1814,9 +1865,8 @@
       <c r="B3" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C3" s="1" t="e">
-        <f>VLOOKUP(A3,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C3" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1826,9 +1876,8 @@
       <c r="B4" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="1" t="e">
-        <f>VLOOKUP(A4,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C4" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,9 +1887,8 @@
       <c r="B5" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C5" s="1" t="e">
-        <f>VLOOKUP(A5,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C5" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,9 +1898,8 @@
       <c r="B6" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="1" t="e">
-        <f>VLOOKUP(A6,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C6" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1862,9 +1909,8 @@
       <c r="B7" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="1" t="e">
-        <f>VLOOKUP(A7,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C7" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1874,9 +1920,8 @@
       <c r="B8" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C8" s="1" t="e">
-        <f>VLOOKUP(A8,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C8" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1886,9 +1931,8 @@
       <c r="B9" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C9" s="1" t="e">
-        <f>VLOOKUP(A9,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C9" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1898,9 +1942,8 @@
       <c r="B10" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="1" t="e">
-        <f>VLOOKUP(A10,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C10" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1910,9 +1953,8 @@
       <c r="B11" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C11" s="1" t="e">
-        <f>VLOOKUP(A11,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C11" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1922,9 +1964,8 @@
       <c r="B12" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C12" s="1" t="e">
-        <f>VLOOKUP(A12,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C12" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1934,9 +1975,8 @@
       <c r="B13" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C13" s="1" t="e">
-        <f>VLOOKUP(A13,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C13" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1946,9 +1986,8 @@
       <c r="B14" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C14" s="1" t="e">
-        <f>VLOOKUP(A14,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
-        <v>#N/A</v>
+      <c r="C14" s="1" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2963,12 +3002,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2976,7 +3015,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
@@ -2984,7 +3023,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B3" t="s">
@@ -2992,7 +3031,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B4" t="s">
@@ -3000,7 +3039,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
@@ -3008,7 +3047,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B6" t="s">
@@ -3016,7 +3055,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B7" t="s">
@@ -3024,7 +3063,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B8" t="s">
@@ -3032,7 +3071,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B9" t="s">
@@ -3040,7 +3079,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B10" t="s">
@@ -3048,7 +3087,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
@@ -3056,7 +3095,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
@@ -3064,7 +3103,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B13" t="s">
@@ -3072,7 +3111,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
@@ -3080,7 +3119,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
@@ -3088,7 +3127,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16" t="s">
@@ -3096,7 +3135,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B17" t="s">
@@ -3104,7 +3143,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
@@ -3112,7 +3151,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
@@ -3120,7 +3159,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
@@ -3128,7 +3167,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
@@ -3136,7 +3175,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
@@ -3144,7 +3183,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B23" t="s">
@@ -3152,7 +3191,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B24" t="s">
@@ -3160,7 +3199,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B25" t="s">
@@ -3168,7 +3207,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B26" t="s">
@@ -3176,7 +3215,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B27" t="s">
@@ -3184,7 +3223,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B28" t="s">
@@ -3192,7 +3231,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B29" t="s">
@@ -3200,7 +3239,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B30" t="s">
@@ -3208,7 +3247,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B31" t="s">
@@ -3216,7 +3255,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B32" t="s">
@@ -3224,7 +3263,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B33" t="s">
@@ -3232,7 +3271,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B34" t="s">
@@ -3240,7 +3279,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B35" t="s">
@@ -3248,7 +3287,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B36" t="s">
@@ -3256,7 +3295,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B37" t="s">
@@ -3264,7 +3303,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B38" t="s">
@@ -3272,7 +3311,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B39" t="s">
@@ -3280,7 +3319,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B40" t="s">
@@ -3288,7 +3327,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
@@ -3296,7 +3335,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B42" t="s">
@@ -3304,7 +3343,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B43" t="s">
@@ -3312,7 +3351,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
@@ -3320,7 +3359,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B45" t="s">
@@ -3328,7 +3367,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B46" t="s">
@@ -3336,7 +3375,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B47" t="s">
@@ -3344,7 +3383,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B48" t="s">
@@ -3352,7 +3391,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B49" t="s">
@@ -3360,7 +3399,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B50" t="s">
@@ -3368,7 +3407,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B51" t="s">
@@ -3376,7 +3415,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B52" t="s">
@@ -3384,7 +3423,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B53" t="s">
@@ -3392,7 +3431,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B54" t="s">
@@ -3400,7 +3439,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B55" t="s">
@@ -3408,7 +3447,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B56" t="s">
@@ -3416,7 +3455,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B57" t="s">
@@ -3424,7 +3463,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B58" t="s">
@@ -3432,7 +3471,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B59" t="s">
@@ -3440,7 +3479,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B60" t="s">
@@ -3448,7 +3487,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B61" t="s">
@@ -3456,7 +3495,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B62" t="s">
@@ -3464,7 +3503,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B63" t="s">
@@ -3472,7 +3511,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B64" t="s">
@@ -3480,7 +3519,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B65" t="s">
@@ -3488,7 +3527,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B66" t="s">
@@ -3496,7 +3535,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B67" t="s">
@@ -3504,7 +3543,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B68" t="s">
@@ -3512,7 +3551,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B69" t="s">
@@ -3520,7 +3559,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B70" t="s">
@@ -3528,7 +3567,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B71" t="s">
@@ -3536,7 +3575,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B72" t="s">
@@ -3544,7 +3583,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B73" t="s">
@@ -3552,7 +3591,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B74" t="s">
@@ -3560,7 +3599,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B75" t="s">
@@ -3568,7 +3607,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B76" t="s">
@@ -3576,7 +3615,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B77" t="s">
@@ -3584,7 +3623,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B78" t="s">
@@ -3592,7 +3631,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B79" t="s">
@@ -3600,7 +3639,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B80" t="s">
@@ -3608,7 +3647,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B81" t="s">

</xml_diff>

<commit_message>
diagram figure 3 working
</commit_message>
<xml_diff>
--- a/configuration.xlsx
+++ b/configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="22200" windowHeight="10335" tabRatio="804" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22200" windowHeight="10335" tabRatio="804"/>
   </bookViews>
   <sheets>
     <sheet name="test_cities" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="281">
   <si>
     <t>City</t>
   </si>
@@ -869,6 +869,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>to know</t>
   </si>
 </sst>
 </file>
@@ -1196,16 +1199,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1217,75 +1222,75 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
+      <c r="A2" t="s">
+        <v>77</v>
       </c>
       <c r="B2">
-        <v>255593</v>
+        <v>123657</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>295124</v>
+        <v>94957</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4">
-        <v>233474</v>
+        <v>124884</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B5">
-        <v>208917</v>
+        <v>866448</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B6">
-        <v>1048575</v>
+        <v>208917</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B7">
-        <v>866448</v>
+        <v>233474</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>94957</v>
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="B9">
-        <v>124884</v>
+        <v>1048575</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>77</v>
+      <c r="A10" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>123657</v>
+        <v>1048575</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1294,14 +1299,6 @@
       </c>
       <c r="B11">
         <v>91137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12">
-        <v>485482</v>
       </c>
     </row>
   </sheetData>
@@ -1314,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A12"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,58 +1759,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
+      <c r="A3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1825,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
increasign values of testing data
</commit_message>
<xml_diff>
--- a/configuration.xlsx
+++ b/configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="22200" windowHeight="10335" tabRatio="804"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22200" windowHeight="10335" tabRatio="804" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test_cities" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="cities_with_energy_data" sheetId="2" r:id="rId4"/>
     <sheet name="cities_with_future_weather" sheetId="4" r:id="rId5"/>
     <sheet name="weather stations" sheetId="5" r:id="rId6"/>
+    <sheet name="configuration2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="380">
   <si>
     <t>City</t>
   </si>
@@ -872,6 +873,303 @@
   </si>
   <si>
     <t>to know</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>Chula Vista CA</t>
+  </si>
+  <si>
+    <t>Oceanside CA</t>
+  </si>
+  <si>
+    <t>Escondido CA</t>
+  </si>
+  <si>
+    <t>Carlsbad CA</t>
+  </si>
+  <si>
+    <t>El Cajon CA</t>
+  </si>
+  <si>
+    <t>Gainesville FL</t>
+  </si>
+  <si>
+    <t>San Marcos CA</t>
+  </si>
+  <si>
+    <t>Vista CA</t>
+  </si>
+  <si>
+    <t>La Jolla CA</t>
+  </si>
+  <si>
+    <t>Encinitas CA</t>
+  </si>
+  <si>
+    <t>Poway CA</t>
+  </si>
+  <si>
+    <t>La Mesa CA</t>
+  </si>
+  <si>
+    <t>Fallbrook CA</t>
+  </si>
+  <si>
+    <t>San Diego CA</t>
+  </si>
+  <si>
+    <t>Seattle WA</t>
+  </si>
+  <si>
+    <t>San Jose CA</t>
+  </si>
+  <si>
+    <t>Houston TX</t>
+  </si>
+  <si>
+    <t>Dallas TX</t>
+  </si>
+  <si>
+    <t>San Francisco CA</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>Los Angeles CA</t>
+  </si>
+  <si>
+    <t>Boston MA</t>
+  </si>
+  <si>
+    <t>Chicago IL</t>
+  </si>
+  <si>
+    <t>Miami FL</t>
+  </si>
+  <si>
+    <t>New York NY</t>
+  </si>
+  <si>
+    <t>Abilene TX</t>
+  </si>
+  <si>
+    <t>Albuquerque NM</t>
+  </si>
+  <si>
+    <t>Ann Arbor MI</t>
+  </si>
+  <si>
+    <t>Austin TX</t>
+  </si>
+  <si>
+    <t>Bellingham WA</t>
+  </si>
+  <si>
+    <t>Bloomington IN</t>
+  </si>
+  <si>
+    <t>Boulder CO</t>
+  </si>
+  <si>
+    <t>Burlington VT</t>
+  </si>
+  <si>
+    <t>Cape Coral FL</t>
+  </si>
+  <si>
+    <t>Champaign IL</t>
+  </si>
+  <si>
+    <t>College Station TX</t>
+  </si>
+  <si>
+    <t>Denver CO</t>
+  </si>
+  <si>
+    <t>Des Moines IA</t>
+  </si>
+  <si>
+    <t>Detroit MI</t>
+  </si>
+  <si>
+    <t>Evansville IN</t>
+  </si>
+  <si>
+    <t>Fayetteville AR</t>
+  </si>
+  <si>
+    <t>Flagstaff AZ</t>
+  </si>
+  <si>
+    <t>Fort Collins CO</t>
+  </si>
+  <si>
+    <t>Grand Junction CO</t>
+  </si>
+  <si>
+    <t>Greeley CO</t>
+  </si>
+  <si>
+    <t>Honolulu HI</t>
+  </si>
+  <si>
+    <t>Indianapolis IN</t>
+  </si>
+  <si>
+    <t>Louisville KY</t>
+  </si>
+  <si>
+    <t>Lynchburg VA</t>
+  </si>
+  <si>
+    <t>Milwaukee WI</t>
+  </si>
+  <si>
+    <t>Minneapolis MN</t>
+  </si>
+  <si>
+    <t>Monroe MI</t>
+  </si>
+  <si>
+    <t>Omaha NE</t>
+  </si>
+  <si>
+    <t>Philadelphia PA</t>
+  </si>
+  <si>
+    <t>Portland OR</t>
+  </si>
+  <si>
+    <t>Roanoke VA</t>
+  </si>
+  <si>
+    <t>Montgomery AL</t>
+  </si>
+  <si>
+    <t>Juneau AK</t>
+  </si>
+  <si>
+    <t>Phoenix AZ</t>
+  </si>
+  <si>
+    <t>Little Rock AR</t>
+  </si>
+  <si>
+    <t>Sacramento CA</t>
+  </si>
+  <si>
+    <t>Hartford CT</t>
+  </si>
+  <si>
+    <t>Dover DE</t>
+  </si>
+  <si>
+    <t>Tallahassee FL</t>
+  </si>
+  <si>
+    <t>Atlanta GA</t>
+  </si>
+  <si>
+    <t>Boise ID</t>
+  </si>
+  <si>
+    <t>Springfield IL</t>
+  </si>
+  <si>
+    <t>Topeka KS</t>
+  </si>
+  <si>
+    <t>Frankfort KY</t>
+  </si>
+  <si>
+    <t>Augusta ME</t>
+  </si>
+  <si>
+    <t>Annapolis MD</t>
+  </si>
+  <si>
+    <t>Lansing MI</t>
+  </si>
+  <si>
+    <t>Saint Paul MN</t>
+  </si>
+  <si>
+    <t>Jackson MS</t>
+  </si>
+  <si>
+    <t>Jefferson City MO</t>
+  </si>
+  <si>
+    <t>Lincoln NE</t>
+  </si>
+  <si>
+    <t>Carson City NV</t>
+  </si>
+  <si>
+    <t>Concord NH</t>
+  </si>
+  <si>
+    <t>Trenton NJ</t>
+  </si>
+  <si>
+    <t>Santa Fe NM</t>
+  </si>
+  <si>
+    <t>Albany NY</t>
+  </si>
+  <si>
+    <t>Raleigh NC</t>
+  </si>
+  <si>
+    <t>Bismarck ND</t>
+  </si>
+  <si>
+    <t>Columbus OH</t>
+  </si>
+  <si>
+    <t>Oklahoma City OK</t>
+  </si>
+  <si>
+    <t>Salem OR</t>
+  </si>
+  <si>
+    <t>Harrisburg PA</t>
+  </si>
+  <si>
+    <t>Providence RI</t>
+  </si>
+  <si>
+    <t>Columbia SC</t>
+  </si>
+  <si>
+    <t>Nashville TN</t>
+  </si>
+  <si>
+    <t>Salt Lake City UT</t>
+  </si>
+  <si>
+    <t>Richmond VA</t>
+  </si>
+  <si>
+    <t>Olympia WA</t>
+  </si>
+  <si>
+    <t>Charleston WV</t>
+  </si>
+  <si>
+    <t>Madison WI</t>
+  </si>
+  <si>
+    <t>Cheyenne WY</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -1201,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,9 +2084,10 @@
     <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1798,8 +2097,14 @@
       <c r="C1" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -1809,8 +2114,14 @@
       <c r="C2" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>32.636099999999999</v>
+      </c>
+      <c r="E2">
+        <v>-117.0532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>101</v>
       </c>
@@ -1820,8 +2131,14 @@
       <c r="C3" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>33.200400000000002</v>
+      </c>
+      <c r="E3">
+        <v>-117.2907</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
@@ -1831,8 +2148,14 @@
       <c r="C4" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>33.119199999999999</v>
+      </c>
+      <c r="E4">
+        <v>-117.0864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>99</v>
       </c>
@@ -1842,8 +2165,14 @@
       <c r="C5" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>33.095799999999997</v>
+      </c>
+      <c r="E5">
+        <v>-117.27209999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
@@ -1853,8 +2182,14 @@
       <c r="C6" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>32.795200000000001</v>
+      </c>
+      <c r="E6">
+        <v>-116.9671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -1864,8 +2199,14 @@
       <c r="C7" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>29.685099999999998</v>
+      </c>
+      <c r="E7">
+        <v>-82.432400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>96</v>
       </c>
@@ -1875,8 +2216,14 @@
       <c r="C8" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>33.156500000000001</v>
+      </c>
+      <c r="E8">
+        <v>-117.1707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>95</v>
       </c>
@@ -1886,8 +2233,14 @@
       <c r="C9" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>33.182000000000002</v>
+      </c>
+      <c r="E9">
+        <v>-117.24679999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
@@ -1897,8 +2250,14 @@
       <c r="C10" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>32.866700000000002</v>
+      </c>
+      <c r="E10">
+        <v>-117.24809999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>93</v>
       </c>
@@ -1908,8 +2267,14 @@
       <c r="C11" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>33.0501</v>
+      </c>
+      <c r="E11">
+        <v>-117.25279999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
@@ -1919,8 +2284,14 @@
       <c r="C12" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>32.977499999999999</v>
+      </c>
+      <c r="E12">
+        <v>-117.0232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>91</v>
       </c>
@@ -1930,8 +2301,14 @@
       <c r="C13" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>32.759599999999999</v>
+      </c>
+      <c r="E13">
+        <v>-116.994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>90</v>
       </c>
@@ -1941,8 +2318,14 @@
       <c r="C14" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>33.398899999999998</v>
+      </c>
+      <c r="E14">
+        <v>-117.2957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -1953,8 +2336,14 @@
         <f>VLOOKUP(A15,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>San_Diego_US-hour</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>32.901400000000002</v>
+      </c>
+      <c r="E15">
+        <v>-117.2079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -1965,8 +2354,14 @@
         <f>VLOOKUP(A16,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Seattle_WA-hour</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>47.602600000000002</v>
+      </c>
+      <c r="E16">
+        <v>-122.3284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -1977,8 +2372,14 @@
         <f>VLOOKUP(A17,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>San_Jose_US-hour</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>37.323900000000002</v>
+      </c>
+      <c r="E17">
+        <v>-121.9144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>87</v>
       </c>
@@ -1989,8 +2390,14 @@
         <f>VLOOKUP(A18,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Houston_US-hour</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>29.8688</v>
+      </c>
+      <c r="E18">
+        <v>-95.537999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>88</v>
       </c>
@@ -2001,8 +2408,14 @@
         <f>VLOOKUP(A19,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Dallas_US-hour</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>32.782499999999999</v>
+      </c>
+      <c r="E19">
+        <v>-96.820700000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>84</v>
       </c>
@@ -2013,8 +2426,14 @@
         <f>VLOOKUP(A20,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>San_Francisco_CA-hour</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>37.735300000000002</v>
+      </c>
+      <c r="E20">
+        <v>-122.3732</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>83</v>
       </c>
@@ -2025,8 +2444,14 @@
         <f>VLOOKUP(A21,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Washington_DC-hour</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>38.874899999999997</v>
+      </c>
+      <c r="E21">
+        <v>-77.032499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -2037,8 +2462,14 @@
         <f>VLOOKUP(A22,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Los_Angeles_CA-hour</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>34.0396</v>
+      </c>
+      <c r="E22">
+        <v>-118.26609999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -2049,8 +2480,14 @@
         <f>VLOOKUP(A23,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Boston_MA-hour</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>42.349600000000002</v>
+      </c>
+      <c r="E23">
+        <v>-71.074600000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>77</v>
       </c>
@@ -2061,8 +2498,14 @@
         <f>VLOOKUP(A24,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Chicago_IL-hour</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>41.928800000000003</v>
+      </c>
+      <c r="E24">
+        <v>-87.631500000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2073,8 +2516,14 @@
         <f>VLOOKUP(A25,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Miami_FL-hour</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>25.938800000000001</v>
+      </c>
+      <c r="E25">
+        <v>-80.214399999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2085,8 +2534,14 @@
         <f>VLOOKUP(A26,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>New_York_(Central_Park)-hour</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>40.752800000000001</v>
+      </c>
+      <c r="E26">
+        <v>-73.972499999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2097,8 +2552,14 @@
         <f>VLOOKUP(A27,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Abilene_US-hour</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>32.341799999999999</v>
+      </c>
+      <c r="E27">
+        <v>-99.941400000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -2109,8 +2570,14 @@
         <f>VLOOKUP(A28,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Albuquerque_NM-hour</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>35.0441</v>
+      </c>
+      <c r="E28">
+        <v>-106.8904</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -2121,8 +2588,14 @@
         <f>VLOOKUP(A29,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Ann_Arbor_US-hour</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>42.273400000000002</v>
+      </c>
+      <c r="E29">
+        <v>-83.713300000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -2133,8 +2606,14 @@
         <f>VLOOKUP(A30,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Austin_US-hour</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>30.2058</v>
+      </c>
+      <c r="E30">
+        <v>-97.800200000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -2145,8 +2624,14 @@
         <f>VLOOKUP(A31,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>BELLINGHAM_INTL-hour</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>48.7395</v>
+      </c>
+      <c r="E31">
+        <v>-122.48090000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -2157,8 +2642,14 @@
         <f>VLOOKUP(A32,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Bloomington_IN_Univ_-hour</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>39.079000000000001</v>
+      </c>
+      <c r="E32">
+        <v>-86.617500000000007</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -2169,8 +2660,14 @@
         <f>VLOOKUP(A33,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Boulder_CO-hour</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>40.087800000000001</v>
+      </c>
+      <c r="E33">
+        <v>-105.37350000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -2181,8 +2678,14 @@
         <f>VLOOKUP(A34,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Burlington_VT-hour</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>44.492899999999999</v>
+      </c>
+      <c r="E34">
+        <v>-73.225300000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -2193,8 +2696,14 @@
         <f>VLOOKUP(A35,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>FORT_MYERS_PAGE_FLD-hour</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>26.6356</v>
+      </c>
+      <c r="E35">
+        <v>-82.016400000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
@@ -2205,8 +2714,14 @@
         <f>VLOOKUP(A36,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>CHAMPAIGN_URBANA-hour</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>40.131900000000002</v>
+      </c>
+      <c r="E36">
+        <v>-88.295199999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -2217,8 +2732,14 @@
         <f>VLOOKUP(A37,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>COLLEGE_STATION-hour</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>30.613099999999999</v>
+      </c>
+      <c r="E37">
+        <v>-96.321700000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -2229,8 +2750,14 @@
         <f>VLOOKUP(A38,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Denver_US-hour</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>39.752499999999998</v>
+      </c>
+      <c r="E38">
+        <v>-104.9995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -2241,8 +2768,14 @@
         <f>VLOOKUP(A39,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Des_Moines_IA-hour</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>41.5839</v>
+      </c>
+      <c r="E39">
+        <v>-93.628900000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
@@ -2253,8 +2786,14 @@
         <f>VLOOKUP(A40,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Detroit_US-hour</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>42.367899999999999</v>
+      </c>
+      <c r="E40">
+        <v>-83.138599999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -2265,8 +2804,14 @@
         <f>VLOOKUP(A41,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Evansville_US-hour</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>37.970799999999997</v>
+      </c>
+      <c r="E41">
+        <v>-87.489699999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>18</v>
       </c>
@@ -2277,8 +2822,14 @@
         <f>VLOOKUP(A42,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>36.118899999999996</v>
+      </c>
+      <c r="E42">
+        <v>-93.983999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -2289,8 +2840,14 @@
         <f>VLOOKUP(A43,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Flagstaff_AZ-hour</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>35.198099999999997</v>
+      </c>
+      <c r="E43">
+        <v>-111.65130000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -2301,8 +2858,14 @@
         <f>VLOOKUP(A44,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Fort_Collins_CO-hour</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>40.593899999999998</v>
+      </c>
+      <c r="E44">
+        <v>-105.12560000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
@@ -2313,8 +2876,14 @@
         <f>VLOOKUP(A45,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Grand_Junction_CO-hour</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>39.126399999999997</v>
+      </c>
+      <c r="E45">
+        <v>-108.5363</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
@@ -2325,8 +2894,14 @@
         <f>VLOOKUP(A46,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>GREELEY_WELD_(AWOS)-hour</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>40.3996</v>
+      </c>
+      <c r="E46">
+        <v>-104.8002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -2337,8 +2912,14 @@
         <f>VLOOKUP(A47,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Honolulu_US-hour</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>21.320900000000002</v>
+      </c>
+      <c r="E47">
+        <v>-157.8389</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>24</v>
       </c>
@@ -2349,8 +2930,14 @@
         <f>VLOOKUP(A48,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Indianapolis_IN-hour</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>39.792999999999999</v>
+      </c>
+      <c r="E48">
+        <v>-86.285300000000007</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
@@ -2361,8 +2948,14 @@
         <f>VLOOKUP(A49,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Louisville_US-hour</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>38.085799999999999</v>
+      </c>
+      <c r="E49">
+        <v>-85.849500000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>28</v>
       </c>
@@ -2373,8 +2966,14 @@
         <f>VLOOKUP(A50,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Lynchburg_Airp_VA-hour</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>37.344000000000001</v>
+      </c>
+      <c r="E50">
+        <v>-79.206400000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>78</v>
       </c>
@@ -2385,8 +2984,14 @@
         <f>VLOOKUP(A51,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Milwaukee_WI-hour</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>43.043399999999998</v>
+      </c>
+      <c r="E51">
+        <v>-87.894499999999994</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -2397,8 +3002,14 @@
         <f>VLOOKUP(A52,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Minneapolis_US-hour</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>45.005899999999997</v>
+      </c>
+      <c r="E52">
+        <v>-93.430499999999995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>31</v>
       </c>
@@ -2409,8 +3020,14 @@
         <f>VLOOKUP(A53,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Monroe-hour</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>41.950499999999998</v>
+      </c>
+      <c r="E53">
+        <v>-83.445700000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>34</v>
       </c>
@@ -2421,8 +3038,14 @@
         <f>VLOOKUP(A54,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Omaha_NE-hour</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>41.207900000000002</v>
+      </c>
+      <c r="E54">
+        <v>-96.118300000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>35</v>
       </c>
@@ -2433,8 +3056,14 @@
         <f>VLOOKUP(A55,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Philadelphia_PA-hour</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>39.952399999999997</v>
+      </c>
+      <c r="E55">
+        <v>-75.165300000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>36</v>
       </c>
@@ -2445,8 +3074,14 @@
         <f>VLOOKUP(A56,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Portland_OR-hour</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>45.469099999999997</v>
+      </c>
+      <c r="E56">
+        <v>-122.5535</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>37</v>
       </c>
@@ -2457,8 +3092,14 @@
         <f>VLOOKUP(A57,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Roanoke_VA-hour</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>37.217700000000001</v>
+      </c>
+      <c r="E57">
+        <v>-79.921000000000006</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>38</v>
       </c>
@@ -2469,8 +3110,14 @@
         <f>VLOOKUP(A58,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Montgomery_AL-hour</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>32.3934</v>
+      </c>
+      <c r="E58">
+        <v>-86.322199999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
@@ -2481,8 +3128,14 @@
         <f>VLOOKUP(A59,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Juneau_AK-hour</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>58.301900000000003</v>
+      </c>
+      <c r="E59">
+        <v>-134.41970000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>79</v>
       </c>
@@ -2493,8 +3146,14 @@
         <f>VLOOKUP(A60,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Phoenix_AZ-hour</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>33.558599999999998</v>
+      </c>
+      <c r="E60">
+        <v>-112.0955</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>40</v>
       </c>
@@ -2505,8 +3164,14 @@
         <f>VLOOKUP(A61,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Little_Rock_AR-hour</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>34.746499999999997</v>
+      </c>
+      <c r="E61">
+        <v>-92.289599999999993</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
@@ -2517,8 +3182,14 @@
         <f>VLOOKUP(A62,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Sacramento_US-hour</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>38.551699999999997</v>
+      </c>
+      <c r="E62">
+        <v>-121.45010000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>42</v>
       </c>
@@ -2529,8 +3200,14 @@
         <f>VLOOKUP(A63,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Hartford_US-hour</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>41.768599999999999</v>
+      </c>
+      <c r="E63">
+        <v>-72.674499999999995</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>43</v>
       </c>
@@ -2541,8 +3218,14 @@
         <f>VLOOKUP(A64,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>DOVER_AFB-hour</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>39.181699999999999</v>
+      </c>
+      <c r="E64">
+        <v>-75.597099999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>44</v>
       </c>
@@ -2553,8 +3236,14 @@
         <f>VLOOKUP(A65,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Tallahassee_FL-hour</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>30.580200000000001</v>
+      </c>
+      <c r="E65">
+        <v>-84.126599999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
@@ -2565,8 +3254,14 @@
         <f>VLOOKUP(A66,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Atlanta_GA-hour</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>33.847700000000003</v>
+      </c>
+      <c r="E66">
+        <v>-84.281400000000005</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>82</v>
       </c>
@@ -2577,8 +3272,14 @@
         <f>VLOOKUP(A67,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Boise_ID-hour</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>43.561</v>
+      </c>
+      <c r="E67">
+        <v>-116.2135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>46</v>
       </c>
@@ -2589,8 +3290,14 @@
         <f>VLOOKUP(A68,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Springfield_(Ill_)_US-hour</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>39.801099999999998</v>
+      </c>
+      <c r="E68">
+        <v>-89.650199999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>47</v>
       </c>
@@ -2601,8 +3308,14 @@
         <f>VLOOKUP(A69,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Topeka_US-hour</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>39.037999999999997</v>
+      </c>
+      <c r="E69">
+        <v>-95.727800000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>48</v>
       </c>
@@ -2613,8 +3326,14 @@
         <f>VLOOKUP(A70,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Frankfort_Lock_4_KY-hour</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>38.235700000000001</v>
+      </c>
+      <c r="E70">
+        <v>-84.959199999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>49</v>
       </c>
@@ -2625,8 +3344,14 @@
         <f>VLOOKUP(A71,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>AUGUSTA_AIRPORT_ME-hour</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>44.405099999999997</v>
+      </c>
+      <c r="E71">
+        <v>-69.756699999999995</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>50</v>
       </c>
@@ -2637,8 +3362,14 @@
         <f>VLOOKUP(A72,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>38.987900000000003</v>
+      </c>
+      <c r="E72">
+        <v>-76.545400000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>53</v>
       </c>
@@ -2649,8 +3380,14 @@
         <f>VLOOKUP(A73,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>East_Lansing_MI-hour</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>42.742199999999997</v>
+      </c>
+      <c r="E73">
+        <v>-84.525499999999994</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>52</v>
       </c>
@@ -2661,8 +3398,14 @@
         <f>VLOOKUP(A74,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>SAINT_PAUL_DOWNTOWN-hour</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>45.010100000000001</v>
+      </c>
+      <c r="E74">
+        <v>-93.151899999999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>51</v>
       </c>
@@ -2673,8 +3416,14 @@
         <f>VLOOKUP(A75,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Jackson_MS-hour</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>32.313400000000001</v>
+      </c>
+      <c r="E75">
+        <v>-90.171999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>54</v>
       </c>
@@ -2685,8 +3434,14 @@
         <f>VLOOKUP(A76,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Jefferson_City_Mem_MO-hour</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>38.551600000000001</v>
+      </c>
+      <c r="E76">
+        <v>-92.274500000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>56</v>
       </c>
@@ -2697,8 +3452,14 @@
         <f>VLOOKUP(A77,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Lincoln_US-hour</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>40.817599999999999</v>
+      </c>
+      <c r="E77">
+        <v>-96.711399999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>57</v>
       </c>
@@ -2709,8 +3470,14 @@
         <f>VLOOKUP(A78,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>39.1496</v>
+      </c>
+      <c r="E78">
+        <v>-119.7178</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>58</v>
       </c>
@@ -2721,8 +3488,14 @@
         <f>VLOOKUP(A79,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Concord_Municipal_NH-hour</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>43.208100000000002</v>
+      </c>
+      <c r="E79">
+        <v>-71.537599999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>59</v>
       </c>
@@ -2733,8 +3506,14 @@
         <f>VLOOKUP(A80,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>TRENTON_MERCER_COUNTY_AP_NJ-hour</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>40.264800000000001</v>
+      </c>
+      <c r="E80">
+        <v>-74.824299999999994</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>60</v>
       </c>
@@ -2745,8 +3524,14 @@
         <f>VLOOKUP(A81,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>SANTA_FE_CO_MUNI-hour</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>35.784700000000001</v>
+      </c>
+      <c r="E81">
+        <v>-105.8749</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>61</v>
       </c>
@@ -2757,8 +3542,14 @@
         <f>VLOOKUP(A82,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Albany_NY-hour</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>42.684899999999999</v>
+      </c>
+      <c r="E82">
+        <v>-73.831800000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2769,8 +3560,14 @@
         <f>VLOOKUP(A83,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Raleigh_NC-hour</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>35.818100000000001</v>
+      </c>
+      <c r="E83">
+        <v>-78.563599999999994</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>62</v>
       </c>
@@ -2781,8 +3578,14 @@
         <f>VLOOKUP(A84,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Bismarck_ND-hour</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>46.815899999999999</v>
+      </c>
+      <c r="E84">
+        <v>-100.70610000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>63</v>
       </c>
@@ -2793,8 +3596,14 @@
         <f>VLOOKUP(A85,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Columbus_OH-hour</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>39.892800000000001</v>
+      </c>
+      <c r="E85">
+        <v>-82.958799999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>64</v>
       </c>
@@ -2805,8 +3614,14 @@
         <f>VLOOKUP(A86,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Oklahoma_City_OK-hour</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>35.579799999999999</v>
+      </c>
+      <c r="E86">
+        <v>-97.573099999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>65</v>
       </c>
@@ -2817,8 +3632,14 @@
         <f>VLOOKUP(A87,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Salem_OR-hour</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>44.901600000000002</v>
+      </c>
+      <c r="E87">
+        <v>-122.92230000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>66</v>
       </c>
@@ -2829,8 +3650,14 @@
         <f>VLOOKUP(A88,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Harrisburg_Capital_PA-hour</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>40.276200000000003</v>
+      </c>
+      <c r="E88">
+        <v>-76.788899999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>67</v>
       </c>
@@ -2841,8 +3668,14 @@
         <f>VLOOKUP(A89,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Providence_RI-hour</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>41.819499999999998</v>
+      </c>
+      <c r="E89">
+        <v>-71.410700000000006</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>68</v>
       </c>
@@ -2853,8 +3686,14 @@
         <f>VLOOKUP(A90,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Columbia_SC-hour</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>34.098799999999997</v>
+      </c>
+      <c r="E90">
+        <v>-81.061199999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>70</v>
       </c>
@@ -2865,8 +3704,14 @@
         <f>VLOOKUP(A91,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Nashville_TN-hour</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>36.147300000000001</v>
+      </c>
+      <c r="E91">
+        <v>-86.777000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>71</v>
       </c>
@@ -2877,8 +3722,14 @@
         <f>VLOOKUP(A92,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Salt_Lake_City_UT-hour</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>40.760800000000003</v>
+      </c>
+      <c r="E92">
+        <v>-111.89109999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>81</v>
       </c>
@@ -2889,8 +3740,14 @@
         <f>VLOOKUP(A93,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Richmond_VA-hour</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>37.585799999999999</v>
+      </c>
+      <c r="E93">
+        <v>-77.488799999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>73</v>
       </c>
@@ -2901,8 +3758,14 @@
         <f>VLOOKUP(A94,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Olympia_WA-hour</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>46.944499999999998</v>
+      </c>
+      <c r="E94">
+        <v>-123.0493</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>74</v>
       </c>
@@ -2913,8 +3776,14 @@
         <f>VLOOKUP(A95,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Charleston_WV-hour</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>38.294400000000003</v>
+      </c>
+      <c r="E95">
+        <v>-81.6096</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>75</v>
       </c>
@@ -2925,8 +3794,14 @@
         <f>VLOOKUP(A96,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>Madison_WI-hour</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>43.108199999999997</v>
+      </c>
+      <c r="E96">
+        <v>-89.270600000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>76</v>
       </c>
@@ -2936,6 +3811,12 @@
       <c r="C97" s="1" t="str">
         <f>VLOOKUP(A97,cities_with_future_weather!$A$1:$B$81,2, FALSE)</f>
         <v>CHEYENNE_MUNICIPAL_ARPT_WY-hour</v>
+      </c>
+      <c r="D97">
+        <v>41.103400000000001</v>
+      </c>
+      <c r="E97">
+        <v>-104.9059</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +3830,7 @@
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4022,4 +4903,1090 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2">
+        <v>-117.0532</v>
+      </c>
+      <c r="C2">
+        <v>32.636099999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3">
+        <v>-117.2907</v>
+      </c>
+      <c r="C3">
+        <v>33.200400000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4">
+        <v>-117.0864</v>
+      </c>
+      <c r="C4">
+        <v>33.119199999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5">
+        <v>-117.27209999999999</v>
+      </c>
+      <c r="C5">
+        <v>33.095799999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6">
+        <v>-116.9671</v>
+      </c>
+      <c r="C6">
+        <v>32.795200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B7">
+        <v>-82.432400000000001</v>
+      </c>
+      <c r="C7">
+        <v>29.685099999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B8">
+        <v>-117.1707</v>
+      </c>
+      <c r="C8">
+        <v>33.156500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9">
+        <v>-117.24679999999999</v>
+      </c>
+      <c r="C9">
+        <v>33.182000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10">
+        <v>-117.24809999999999</v>
+      </c>
+      <c r="C10">
+        <v>32.866700000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11">
+        <v>-117.25279999999999</v>
+      </c>
+      <c r="C11">
+        <v>33.0501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12">
+        <v>-117.0232</v>
+      </c>
+      <c r="C12">
+        <v>32.977499999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13">
+        <v>-116.994</v>
+      </c>
+      <c r="C13">
+        <v>32.759599999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14">
+        <v>-117.2957</v>
+      </c>
+      <c r="C14">
+        <v>33.398899999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15">
+        <v>-117.2079</v>
+      </c>
+      <c r="C15">
+        <v>32.901400000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16">
+        <v>-122.3284</v>
+      </c>
+      <c r="C16">
+        <v>47.602600000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B17">
+        <v>-121.9144</v>
+      </c>
+      <c r="C17">
+        <v>37.323900000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18">
+        <v>-95.537999999999997</v>
+      </c>
+      <c r="C18">
+        <v>29.8688</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B19">
+        <v>-96.820700000000002</v>
+      </c>
+      <c r="C19">
+        <v>32.782499999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B20">
+        <v>-122.3732</v>
+      </c>
+      <c r="C20">
+        <v>37.735300000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21">
+        <v>-77.032499999999999</v>
+      </c>
+      <c r="C21">
+        <v>38.874899999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22">
+        <v>-118.26609999999999</v>
+      </c>
+      <c r="C22">
+        <v>34.0396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B23">
+        <v>-71.074600000000004</v>
+      </c>
+      <c r="C23">
+        <v>42.349600000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B24">
+        <v>-87.631500000000003</v>
+      </c>
+      <c r="C24">
+        <v>41.928800000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B25">
+        <v>-80.214399999999998</v>
+      </c>
+      <c r="C25">
+        <v>25.938800000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B26">
+        <v>-73.972499999999997</v>
+      </c>
+      <c r="C26">
+        <v>40.752800000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B27">
+        <v>-99.941400000000002</v>
+      </c>
+      <c r="C27">
+        <v>32.341799999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B28">
+        <v>-106.8904</v>
+      </c>
+      <c r="C28">
+        <v>35.0441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B29">
+        <v>-83.713300000000004</v>
+      </c>
+      <c r="C29">
+        <v>42.273400000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B30">
+        <v>-97.800200000000004</v>
+      </c>
+      <c r="C30">
+        <v>30.2058</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31">
+        <v>-122.48090000000001</v>
+      </c>
+      <c r="C31">
+        <v>48.7395</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B32">
+        <v>-86.617500000000007</v>
+      </c>
+      <c r="C32">
+        <v>39.079000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B33">
+        <v>-105.37350000000001</v>
+      </c>
+      <c r="C33">
+        <v>40.087800000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B34">
+        <v>-73.225300000000004</v>
+      </c>
+      <c r="C34">
+        <v>44.492899999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B35">
+        <v>-82.016400000000004</v>
+      </c>
+      <c r="C35">
+        <v>26.6356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B36">
+        <v>-88.295199999999994</v>
+      </c>
+      <c r="C36">
+        <v>40.131900000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B37">
+        <v>-96.321700000000007</v>
+      </c>
+      <c r="C37">
+        <v>30.613099999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B38">
+        <v>-104.9995</v>
+      </c>
+      <c r="C38">
+        <v>39.752499999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B39">
+        <v>-93.628900000000002</v>
+      </c>
+      <c r="C39">
+        <v>41.5839</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B40">
+        <v>-83.138599999999997</v>
+      </c>
+      <c r="C40">
+        <v>42.367899999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B41">
+        <v>-87.489699999999999</v>
+      </c>
+      <c r="C41">
+        <v>37.970799999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B42">
+        <v>-93.983999999999995</v>
+      </c>
+      <c r="C42">
+        <v>36.118899999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43">
+        <v>-111.65130000000001</v>
+      </c>
+      <c r="C43">
+        <v>35.198099999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B44">
+        <v>-105.12560000000001</v>
+      </c>
+      <c r="C44">
+        <v>40.593899999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B45">
+        <v>-108.5363</v>
+      </c>
+      <c r="C45">
+        <v>39.126399999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B46">
+        <v>-104.8002</v>
+      </c>
+      <c r="C46">
+        <v>40.3996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B47">
+        <v>-157.8389</v>
+      </c>
+      <c r="C47">
+        <v>21.320900000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B48">
+        <v>-86.285300000000007</v>
+      </c>
+      <c r="C48">
+        <v>39.792999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B49">
+        <v>-85.849500000000006</v>
+      </c>
+      <c r="C49">
+        <v>38.085799999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B50">
+        <v>-79.206400000000002</v>
+      </c>
+      <c r="C50">
+        <v>37.344000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B51">
+        <v>-87.894499999999994</v>
+      </c>
+      <c r="C51">
+        <v>43.043399999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B52">
+        <v>-93.430499999999995</v>
+      </c>
+      <c r="C52">
+        <v>45.005899999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B53">
+        <v>-83.445700000000002</v>
+      </c>
+      <c r="C53">
+        <v>41.950499999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B54">
+        <v>-96.118300000000005</v>
+      </c>
+      <c r="C54">
+        <v>41.207900000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B55">
+        <v>-75.165300000000002</v>
+      </c>
+      <c r="C55">
+        <v>39.952399999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B56">
+        <v>-122.5535</v>
+      </c>
+      <c r="C56">
+        <v>45.469099999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B57">
+        <v>-79.921000000000006</v>
+      </c>
+      <c r="C57">
+        <v>37.217700000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B58">
+        <v>-86.322199999999995</v>
+      </c>
+      <c r="C58">
+        <v>32.3934</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B59">
+        <v>-134.41970000000001</v>
+      </c>
+      <c r="C59">
+        <v>58.301900000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B60">
+        <v>-112.0955</v>
+      </c>
+      <c r="C60">
+        <v>33.558599999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B61">
+        <v>-92.289599999999993</v>
+      </c>
+      <c r="C61">
+        <v>34.746499999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B62">
+        <v>-121.45010000000001</v>
+      </c>
+      <c r="C62">
+        <v>38.551699999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B63">
+        <v>-72.674499999999995</v>
+      </c>
+      <c r="C63">
+        <v>41.768599999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B64">
+        <v>-75.597099999999998</v>
+      </c>
+      <c r="C64">
+        <v>39.181699999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B65">
+        <v>-84.126599999999996</v>
+      </c>
+      <c r="C65">
+        <v>30.580200000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B66">
+        <v>-84.281400000000005</v>
+      </c>
+      <c r="C66">
+        <v>33.847700000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B67">
+        <v>-116.2135</v>
+      </c>
+      <c r="C67">
+        <v>43.561</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B68">
+        <v>-89.650199999999998</v>
+      </c>
+      <c r="C68">
+        <v>39.801099999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B69">
+        <v>-95.727800000000002</v>
+      </c>
+      <c r="C69">
+        <v>39.037999999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B70">
+        <v>-84.959199999999996</v>
+      </c>
+      <c r="C70">
+        <v>38.235700000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B71">
+        <v>-69.756699999999995</v>
+      </c>
+      <c r="C71">
+        <v>44.405099999999997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B72">
+        <v>-76.545400000000001</v>
+      </c>
+      <c r="C72">
+        <v>38.987900000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B73">
+        <v>-84.525499999999994</v>
+      </c>
+      <c r="C73">
+        <v>42.742199999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B74">
+        <v>-93.151899999999998</v>
+      </c>
+      <c r="C74">
+        <v>45.010100000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B75">
+        <v>-90.171999999999997</v>
+      </c>
+      <c r="C75">
+        <v>32.313400000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B76">
+        <v>-92.274500000000003</v>
+      </c>
+      <c r="C76">
+        <v>38.551600000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B77">
+        <v>-96.711399999999998</v>
+      </c>
+      <c r="C77">
+        <v>40.817599999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B78">
+        <v>-119.7178</v>
+      </c>
+      <c r="C78">
+        <v>39.1496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B79">
+        <v>-71.537599999999998</v>
+      </c>
+      <c r="C79">
+        <v>43.208100000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B80">
+        <v>-74.824299999999994</v>
+      </c>
+      <c r="C80">
+        <v>40.264800000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B81">
+        <v>-105.8749</v>
+      </c>
+      <c r="C81">
+        <v>35.784700000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B82">
+        <v>-73.831800000000001</v>
+      </c>
+      <c r="C82">
+        <v>42.684899999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B83">
+        <v>-78.563599999999994</v>
+      </c>
+      <c r="C83">
+        <v>35.818100000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B84">
+        <v>-100.70610000000001</v>
+      </c>
+      <c r="C84">
+        <v>46.815899999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B85">
+        <v>-82.958799999999997</v>
+      </c>
+      <c r="C85">
+        <v>39.892800000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B86">
+        <v>-97.573099999999997</v>
+      </c>
+      <c r="C86">
+        <v>35.579799999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B87">
+        <v>-122.92230000000001</v>
+      </c>
+      <c r="C87">
+        <v>44.901600000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B88">
+        <v>-76.788899999999998</v>
+      </c>
+      <c r="C88">
+        <v>40.276200000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B89">
+        <v>-71.410700000000006</v>
+      </c>
+      <c r="C89">
+        <v>41.819499999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B90">
+        <v>-81.061199999999999</v>
+      </c>
+      <c r="C90">
+        <v>34.098799999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B91">
+        <v>-86.777000000000001</v>
+      </c>
+      <c r="C91">
+        <v>36.147300000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B92">
+        <v>-111.89109999999999</v>
+      </c>
+      <c r="C92">
+        <v>40.760800000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B93">
+        <v>-77.488799999999998</v>
+      </c>
+      <c r="C93">
+        <v>37.585799999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B94">
+        <v>-123.0493</v>
+      </c>
+      <c r="C94">
+        <v>46.944499999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B95">
+        <v>-81.6096</v>
+      </c>
+      <c r="C95">
+        <v>38.294400000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B96">
+        <v>-89.270600000000002</v>
+      </c>
+      <c r="C96">
+        <v>43.108199999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B97">
+        <v>-104.9059</v>
+      </c>
+      <c r="C97">
+        <v>41.103400000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>